<commit_message>
update `caravel-5V-dev-v6-M.2` (REV6B) + add an 0.1uF bypass cap to the Flash level shifters ~ update BOM
</commit_message>
<xml_diff>
--- a/hardware/caravel-5V-dev-v6-M.2/caravel-5V-dev-v6-M.2.xlsx
+++ b/hardware/caravel-5V-dev-v6-M.2/caravel-5V-dev-v6-M.2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
   <si>
     <t xml:space="preserve">Designators</t>
   </si>
@@ -73,10 +73,10 @@
     <t xml:space="preserve">TAR5S33UTE85LF</t>
   </si>
   <si>
-    <t xml:space="preserve">U6, U9, U10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TXB0104PWR</t>
+    <t xml:space="preserve">U6, U9, U10, U11, U12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN74LV1T34DCKR</t>
   </si>
   <si>
     <t xml:space="preserve">U7</t>
@@ -100,43 +100,52 @@
     <t xml:space="preserve">LTST-C230KRKT</t>
   </si>
   <si>
-    <t xml:space="preserve">C12. C14</t>
+    <t xml:space="preserve">C12. C19, C20</t>
   </si>
   <si>
     <t xml:space="preserve">10u</t>
   </si>
   <si>
-    <t xml:space="preserve">CC0805KKX5R8BB106</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C10</t>
+    <t xml:space="preserve">CL21B106KAYQNNE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C10, C18</t>
   </si>
   <si>
     <t xml:space="preserve">1u</t>
   </si>
   <si>
-    <t xml:space="preserve">CC0805KKX7R7BB105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C2-C9, C13, C15-C22</t>
+    <t xml:space="preserve">885012207103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2-C9, C14-C16,C21-C23</t>
   </si>
   <si>
     <t xml:space="preserve">0.1u</t>
   </si>
   <si>
-    <t xml:space="preserve">CC0805KRX7R9BB104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C11</t>
+    <t xml:space="preserve">C0805C104K5RAC7411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1, C11, C13, C17</t>
   </si>
   <si>
     <t xml:space="preserve">0.01u</t>
   </si>
   <si>
-    <t xml:space="preserve">CC0805JRX7R9BB103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R1, R5-R12, R15-R18</t>
+    <t xml:space="preserve">C0805C103K5RAC7411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7, R8, R10, R11, R20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0805FR-07100KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1, R5, R6, R9, R12-R17, R19</t>
   </si>
   <si>
     <t xml:space="preserve">10K</t>
@@ -154,13 +163,13 @@
     <t xml:space="preserve">RMCF0805FT12K0</t>
   </si>
   <si>
-    <t xml:space="preserve">R13, R14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0805FR-071KL</t>
+    <t xml:space="preserve">R18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0805FR-072KL</t>
   </si>
   <si>
     <t xml:space="preserve">R3, R4</t>
@@ -197,6 +206,30 @@
   </si>
   <si>
     <t xml:space="preserve">36-5000-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FB1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">600R @ 100MHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7427920415</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKQGADE010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alps Alpine </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRLML6402TRPBF</t>
   </si>
 </sst>
 </file>
@@ -430,16 +463,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.58"/>
   </cols>
@@ -525,13 +559,13 @@
         <v>17</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G6" s="6"/>
     </row>
@@ -582,7 +616,7 @@
         <v>26</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>27</v>
@@ -591,7 +625,7 @@
         <v>28</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -599,7 +633,7 @@
         <v>29</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>30</v>
@@ -608,7 +642,7 @@
         <v>31</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -616,7 +650,7 @@
         <v>32</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>33</v>
@@ -625,7 +659,7 @@
         <v>34</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -633,7 +667,7 @@
         <v>35</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>36</v>
@@ -642,7 +676,7 @@
         <v>37</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -650,7 +684,7 @@
         <v>38</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>39</v>
@@ -667,7 +701,7 @@
         <v>41</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>42</v>
@@ -701,13 +735,13 @@
         <v>47</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C17" s="7" t="n">
-        <v>150</v>
-      </c>
-      <c r="D17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>48</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>49</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>14</v>
@@ -715,13 +749,16 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C18" s="7" t="n">
+        <v>150</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>14</v>
@@ -729,15 +766,12 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="6" t="s">
         <v>53</v>
       </c>
       <c r="E19" s="0" t="s">
@@ -766,37 +800,105 @@
         <v>57</v>
       </c>
       <c r="B21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="D22" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" display="SN74LVC1G125DCKT"/>
     <hyperlink ref="D4" r:id="rId2" display="MCP1319MT-29LE/OT"/>
     <hyperlink ref="D5" r:id="rId3" display="TAR5S33UTE85LF"/>
-    <hyperlink ref="D6" r:id="rId4" display="TXB0104PWR"/>
+    <hyperlink ref="D6" r:id="rId4" display="SN74LV1T34DCKR"/>
     <hyperlink ref="D7" r:id="rId5" display="W25Q32JVSSIQ"/>
     <hyperlink ref="D8" r:id="rId6" display="M.2 E connector"/>
     <hyperlink ref="D9" r:id="rId7" display="LTST-C230KRKT"/>
-    <hyperlink ref="D10" r:id="rId8" display="CC0805KKX5R8BB106"/>
-    <hyperlink ref="D11" r:id="rId9" display="CC0805KKX7R7BB105"/>
-    <hyperlink ref="D12" r:id="rId10" display="CC0805KRX7R9BB104"/>
-    <hyperlink ref="D13" r:id="rId11" display="CC0805JRX7R9BB103"/>
-    <hyperlink ref="D14" r:id="rId12" display="RC0805FR-0710KL"/>
-    <hyperlink ref="D15" r:id="rId13" display="RMCF0805FT12K0"/>
-    <hyperlink ref="D16" r:id="rId14" display="RC0805FR-071KL"/>
-    <hyperlink ref="D17" r:id="rId15" display="RNCP0805FTD150R"/>
-    <hyperlink ref="D18" r:id="rId16" display="10118193-0001LF"/>
-    <hyperlink ref="D19" r:id="rId17" display="SG7050CCN-10-000000M-HJGA3"/>
-    <hyperlink ref="D20" r:id="rId18" display="CSTNE12M0GH5L000R0"/>
-    <hyperlink ref="D21" r:id="rId19" display="36-5000-ND"/>
+    <hyperlink ref="D10" r:id="rId8" display="CL21B106KAYQNNE"/>
+    <hyperlink ref="D11" r:id="rId9" display="885012207103"/>
+    <hyperlink ref="D12" r:id="rId10" display="C0805C104K5RAC7411"/>
+    <hyperlink ref="D13" r:id="rId11" display="C0805C103K5RAC7411"/>
+    <hyperlink ref="D14" r:id="rId12" display="RC0805FR-07100KL"/>
+    <hyperlink ref="D15" r:id="rId13" display="RC0805FR-0710KL"/>
+    <hyperlink ref="D16" r:id="rId14" display="RMCF0805FT12K0"/>
+    <hyperlink ref="D17" r:id="rId15" display="RC0805FR-072KL"/>
+    <hyperlink ref="D18" r:id="rId16" display="RNCP0805FTD150R"/>
+    <hyperlink ref="D19" r:id="rId17" display="10118193-0001LF"/>
+    <hyperlink ref="D20" r:id="rId18" display="SG7050CCN-10-000000M-HJGA3"/>
+    <hyperlink ref="D21" r:id="rId19" display="CSTNE12M0GH5L000R0"/>
+    <hyperlink ref="D22" r:id="rId20" display="36-5000-ND"/>
+    <hyperlink ref="D23" r:id="rId21" display="7427920415"/>
+    <hyperlink ref="D24" r:id="rId22" display="SKQGADE010"/>
+    <hyperlink ref="D25" r:id="rId23" display="IRLML6402TRPBF"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>